<commit_message>
Adds new tables and serveys
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF/forms/MIF/MIF.xlsx
+++ b/app/config/tables/MIF/forms/MIF/MIF.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98DAFE6-4208-41AC-8890-484C9A0510FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C351D-4FEC-4E42-BDC3-2BD467092E4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="367">
   <si>
     <t>setting_name</t>
   </si>
@@ -826,270 +826,6 @@
   </si>
   <si>
     <t>CONSENTFOR</t>
-  </si>
-  <si>
-    <t>tab1</t>
-  </si>
-  <si>
-    <t>tab2</t>
-  </si>
-  <si>
-    <t>tab5</t>
-  </si>
-  <si>
-    <t>Ntchugal</t>
-  </si>
-  <si>
-    <t>Blas</t>
-  </si>
-  <si>
-    <t>Colicunda</t>
-  </si>
-  <si>
-    <t>Wanquilim</t>
-  </si>
-  <si>
-    <t>Mandingara</t>
-  </si>
-  <si>
-    <t>Cutia</t>
-  </si>
-  <si>
-    <t>Rossum</t>
-  </si>
-  <si>
-    <t>Amedalae</t>
-  </si>
-  <si>
-    <t>Ntchane</t>
-  </si>
-  <si>
-    <t>Quinhaque Mansoa</t>
-  </si>
-  <si>
-    <t>Ntchangue Bideta</t>
-  </si>
-  <si>
-    <t>Ntchangue Subal</t>
-  </si>
-  <si>
-    <t>Jogudul Com</t>
-  </si>
-  <si>
-    <t>Joaquim Com</t>
-  </si>
-  <si>
-    <t>Cangha Ntchugal</t>
-  </si>
-  <si>
-    <t>Cangha Cocry</t>
-  </si>
-  <si>
-    <t>Encheia</t>
-  </si>
-  <si>
-    <t>Cadjque</t>
-  </si>
-  <si>
-    <t>Mpas</t>
-  </si>
-  <si>
-    <t>Quinhaque Ncor</t>
-  </si>
-  <si>
-    <t>Quinhaque</t>
-  </si>
-  <si>
-    <t>Untche</t>
-  </si>
-  <si>
-    <t>Cumbidjam</t>
-  </si>
-  <si>
-    <t>Sintcham</t>
-  </si>
-  <si>
-    <t>Sansancutoto</t>
-  </si>
-  <si>
-    <t>Bironque</t>
-  </si>
-  <si>
-    <t>Gendo</t>
-  </si>
-  <si>
-    <t>Mansaba</t>
-  </si>
-  <si>
-    <t>Sanaia</t>
-  </si>
-  <si>
-    <t>Galenque</t>
-  </si>
-  <si>
-    <t>Demba So</t>
-  </si>
-  <si>
-    <t>Bilma</t>
-  </si>
-  <si>
-    <t>Gua</t>
-  </si>
-  <si>
-    <t>Ntusse</t>
-  </si>
-  <si>
-    <t>Ponta Vicente</t>
-  </si>
-  <si>
-    <t>Incaite</t>
-  </si>
-  <si>
-    <t>Qindinga</t>
-  </si>
-  <si>
-    <t>Intuzinho</t>
-  </si>
-  <si>
-    <t>Bambadinca</t>
-  </si>
-  <si>
-    <t>Iem</t>
-  </si>
-  <si>
-    <t>Buno</t>
-  </si>
-  <si>
-    <t>Prite</t>
-  </si>
-  <si>
-    <t>Reino Quicete</t>
-  </si>
-  <si>
-    <t>Betafte</t>
-  </si>
-  <si>
-    <t>Bissa</t>
-  </si>
-  <si>
-    <t>Reino Tor</t>
-  </si>
-  <si>
-    <t>Dorse</t>
-  </si>
-  <si>
-    <t>Blim Blim</t>
-  </si>
-  <si>
-    <t>Quinsana</t>
-  </si>
-  <si>
-    <t>Quita</t>
-  </si>
-  <si>
-    <t>Ondame</t>
-  </si>
-  <si>
-    <t>Blom</t>
-  </si>
-  <si>
-    <t>Bocomul</t>
-  </si>
-  <si>
-    <t>Ome</t>
-  </si>
-  <si>
-    <t>Quinhamel</t>
-  </si>
-  <si>
-    <t>Ponta Augusto Vicente</t>
-  </si>
-  <si>
-    <t>Bilmate</t>
-  </si>
-  <si>
-    <t>Badjefa</t>
-  </si>
-  <si>
-    <t>Gundjur</t>
-  </si>
-  <si>
-    <t>Carabele</t>
-  </si>
-  <si>
-    <t>Nema</t>
-  </si>
-  <si>
-    <t>Dobanla</t>
-  </si>
-  <si>
-    <t>Sintcham Delo Mamado</t>
-  </si>
-  <si>
-    <t>"      "     "    "    "  Malam</t>
-  </si>
-  <si>
-    <t>"     "      " Umaro</t>
-  </si>
-  <si>
-    <t>Ponhe Maunde</t>
-  </si>
-  <si>
-    <t>Candjufa</t>
-  </si>
-  <si>
-    <t>Olocunda</t>
-  </si>
-  <si>
-    <t>Funtufuntula</t>
-  </si>
-  <si>
-    <t>Sintcham Iero Djadja</t>
-  </si>
-  <si>
-    <t>Buruntuma</t>
-  </si>
-  <si>
-    <t>Dara Braima</t>
-  </si>
-  <si>
-    <t>Padjama</t>
-  </si>
-  <si>
-    <t>Sintcham Cunadi(Camedina)</t>
-  </si>
-  <si>
-    <t>Djebacunda</t>
-  </si>
-  <si>
-    <t>Afia</t>
-  </si>
-  <si>
-    <t>Camanca</t>
-  </si>
-  <si>
-    <t>Fasse(Bairo Ii)</t>
-  </si>
-  <si>
-    <t>Mafonco</t>
-  </si>
-  <si>
-    <t>Samba Canda</t>
-  </si>
-  <si>
-    <t>Sintcham Nhapo</t>
-  </si>
-  <si>
-    <t>Tabadjenque</t>
-  </si>
-  <si>
-    <t>Tchetche</t>
-  </si>
-  <si>
-    <t>Sintcham Cunadi (Camedina)</t>
-  </si>
-  <si>
-    <t>Fasse (Bairo Ii)</t>
   </si>
   <si>
     <t>query_name</t>
@@ -1392,6 +1128,21 @@
   </si>
   <si>
     <t>Makes the date widget DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>data('CESCO') == '1'</t>
+  </si>
+  <si>
+    <t>What grade?</t>
+  </si>
+  <si>
+    <t>ESCONS</t>
+  </si>
+  <si>
+    <t>Have you ever attended school</t>
+  </si>
+  <si>
+    <t>Número de mulher</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1268,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1537,7 +1288,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1941,11 +1691,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:R101"/>
+  <dimension ref="A1:R108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="G15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +1741,7 @@
         <v>173</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>361</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2005,7 +1755,7 @@
         <v>121</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>357</v>
+        <v>269</v>
       </c>
       <c r="F3" t="s">
         <v>122</v>
@@ -2022,7 +1772,7 @@
         <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>360</v>
+        <v>272</v>
       </c>
       <c r="F4" t="s">
         <v>125</v>
@@ -2033,8 +1783,8 @@
       <c r="H4" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="J4" s="19" t="s">
-        <v>366</v>
+      <c r="J4" s="18" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2050,7 +1800,7 @@
       <c r="H5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="J5" s="19"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
@@ -2150,10 +1900,12 @@
       <c r="F15" t="s">
         <v>135</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -2166,8 +1918,8 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="22" t="s">
-        <v>447</v>
+      <c r="D18" s="21" t="s">
+        <v>359</v>
       </c>
       <c r="F18" t="s">
         <v>140</v>
@@ -2181,13 +1933,13 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>430</v>
+        <v>342</v>
       </c>
       <c r="E19" t="s">
-        <v>431</v>
+        <v>343</v>
       </c>
       <c r="F19" t="s">
-        <v>433</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -2195,7 +1947,7 @@
         <v>156</v>
       </c>
       <c r="C20" t="s">
-        <v>434</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -2265,13 +2017,13 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>430</v>
+        <v>342</v>
       </c>
       <c r="E28" t="s">
-        <v>431</v>
+        <v>343</v>
       </c>
       <c r="F28" t="s">
-        <v>435</v>
+        <v>347</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -2320,18 +2072,18 @@
         <v>153</v>
       </c>
       <c r="H33" t="s">
-        <v>364</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>430</v>
+        <v>342</v>
       </c>
       <c r="E34" t="s">
-        <v>431</v>
+        <v>343</v>
       </c>
       <c r="F34" t="s">
-        <v>436</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
@@ -2474,7 +2226,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>156</v>
       </c>
@@ -2485,7 +2237,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>163</v>
       </c>
@@ -2496,7 +2248,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>164</v>
       </c>
@@ -2504,7 +2256,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>163</v>
       </c>
@@ -2515,416 +2267,412 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D56" s="22" t="s">
-        <v>447</v>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>143</v>
+      </c>
+      <c r="E56" t="s">
+        <v>34</v>
       </c>
       <c r="F56" t="s">
+        <v>280</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" t="s">
+        <v>281</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>342</v>
+      </c>
+      <c r="E59" t="s">
+        <v>343</v>
+      </c>
+      <c r="F59" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D63" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="F63" t="s">
         <v>174</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G63" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H63" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>29</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F64" t="s">
         <v>177</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G64" t="s">
         <v>177</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H64" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="B58" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
-      <c r="B59" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="B66" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>211</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G67" t="s">
         <v>213</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H67" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>143</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E68" t="s">
         <v>38</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F68" t="s">
         <v>214</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G68" t="s">
         <v>210</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H68" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>156</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C69" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
         <v>143</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E70" t="s">
         <v>41</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F70" t="s">
         <v>215</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G70" t="s">
         <v>216</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H70" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>156</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C72" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
         <v>163</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F73" t="s">
         <v>208</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I73" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
         <v>163</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F75" t="s">
         <v>208</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I75" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
         <v>29</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F79" t="s">
         <v>179</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G79" t="s">
         <v>180</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H79" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>430</v>
-      </c>
-      <c r="E73" t="s">
-        <v>431</v>
-      </c>
-      <c r="F73" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>29</v>
-      </c>
-      <c r="F74" t="s">
-        <v>182</v>
-      </c>
-      <c r="G74" t="s">
-        <v>183</v>
-      </c>
-      <c r="H74" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>430</v>
-      </c>
-      <c r="E75" t="s">
-        <v>431</v>
-      </c>
-      <c r="F75" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>29</v>
-      </c>
-      <c r="F76" t="s">
-        <v>185</v>
-      </c>
-      <c r="G76" t="s">
-        <v>186</v>
-      </c>
-      <c r="H76" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>430</v>
-      </c>
-      <c r="E77" t="s">
-        <v>431</v>
-      </c>
-      <c r="F77" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>29</v>
+        <v>342</v>
+      </c>
+      <c r="E80" t="s">
+        <v>343</v>
       </c>
       <c r="F80" t="s">
-        <v>188</v>
-      </c>
-      <c r="G80" t="s">
-        <v>192</v>
-      </c>
-      <c r="H80" t="s">
-        <v>189</v>
+        <v>349</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>430</v>
-      </c>
-      <c r="E81" t="s">
-        <v>431</v>
+        <v>29</v>
       </c>
       <c r="F81" t="s">
-        <v>440</v>
+        <v>182</v>
+      </c>
+      <c r="G81" t="s">
+        <v>183</v>
+      </c>
+      <c r="H81" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>29</v>
+        <v>342</v>
+      </c>
+      <c r="E82" t="s">
+        <v>343</v>
       </c>
       <c r="F82" t="s">
-        <v>190</v>
-      </c>
-      <c r="G82" t="s">
-        <v>193</v>
-      </c>
-      <c r="H82" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
-        <v>430</v>
-      </c>
-      <c r="E83" t="s">
-        <v>431</v>
+        <v>29</v>
       </c>
       <c r="F83" t="s">
-        <v>441</v>
+        <v>185</v>
+      </c>
+      <c r="G83" t="s">
+        <v>186</v>
+      </c>
+      <c r="H83" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>15</v>
+      <c r="D84" t="s">
+        <v>342</v>
+      </c>
+      <c r="E84" t="s">
+        <v>343</v>
+      </c>
+      <c r="F84" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>143</v>
-      </c>
-      <c r="E86" t="s">
-        <v>34</v>
-      </c>
-      <c r="F86" t="s">
-        <v>194</v>
-      </c>
-      <c r="G86" t="s">
-        <v>195</v>
-      </c>
-      <c r="H86" t="s">
-        <v>196</v>
-      </c>
-    </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>156</v>
-      </c>
-      <c r="C87" t="s">
-        <v>224</v>
+      <c r="D87" t="s">
+        <v>29</v>
+      </c>
+      <c r="F87" t="s">
+        <v>188</v>
+      </c>
+      <c r="G87" t="s">
+        <v>192</v>
+      </c>
+      <c r="H87" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
-        <v>131</v>
+        <v>342</v>
+      </c>
+      <c r="E88" t="s">
+        <v>343</v>
       </c>
       <c r="F88" t="s">
-        <v>197</v>
-      </c>
-      <c r="G88" t="s">
-        <v>198</v>
-      </c>
-      <c r="H88" t="s">
-        <v>199</v>
+        <v>352</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>161</v>
+      <c r="D89" t="s">
+        <v>29</v>
+      </c>
+      <c r="F89" t="s">
+        <v>190</v>
+      </c>
+      <c r="G89" t="s">
+        <v>193</v>
+      </c>
+      <c r="H89" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>15</v>
+      <c r="D90" t="s">
+        <v>342</v>
+      </c>
+      <c r="E90" t="s">
+        <v>343</v>
+      </c>
+      <c r="F90" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
         <v>143</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E93" t="s">
         <v>34</v>
       </c>
-      <c r="F92" t="s">
-        <v>200</v>
-      </c>
-      <c r="G92" t="s">
-        <v>201</v>
-      </c>
-      <c r="H92" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+      <c r="F93" t="s">
+        <v>194</v>
+      </c>
+      <c r="G93" t="s">
+        <v>195</v>
+      </c>
+      <c r="H93" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
         <v>156</v>
       </c>
-      <c r="C93" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
-        <v>29</v>
-      </c>
-      <c r="F94" t="s">
-        <v>202</v>
-      </c>
-      <c r="G94" t="s">
-        <v>203</v>
-      </c>
-      <c r="H94" t="s">
-        <v>204</v>
+      <c r="C94" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D95" t="s">
-        <v>430</v>
-      </c>
-      <c r="E95" t="s">
-        <v>431</v>
+        <v>131</v>
       </c>
       <c r="F95" t="s">
-        <v>443</v>
+        <v>197</v>
+      </c>
+      <c r="G95" t="s">
+        <v>198</v>
+      </c>
+      <c r="H95" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
@@ -2944,32 +2692,97 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
+        <v>143</v>
+      </c>
+      <c r="E99" t="s">
+        <v>34</v>
+      </c>
+      <c r="F99" t="s">
+        <v>200</v>
+      </c>
+      <c r="G99" t="s">
+        <v>201</v>
+      </c>
+      <c r="H99" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>156</v>
+      </c>
+      <c r="C100" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
         <v>29</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F101" t="s">
+        <v>202</v>
+      </c>
+      <c r="G101" t="s">
+        <v>203</v>
+      </c>
+      <c r="H101" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>342</v>
+      </c>
+      <c r="E102" t="s">
+        <v>343</v>
+      </c>
+      <c r="F102" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>29</v>
+      </c>
+      <c r="F106" t="s">
         <v>205</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G106" t="s">
         <v>207</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H106" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
-        <v>430</v>
-      </c>
-      <c r="E100" t="s">
-        <v>431</v>
-      </c>
-      <c r="F100" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
-      <c r="B101" t="s">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>342</v>
+      </c>
+      <c r="E107" t="s">
+        <v>343</v>
+      </c>
+      <c r="F107" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="11"/>
+      <c r="B108" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2996,57 +2809,57 @@
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>354</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>355</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>363</v>
+    <row r="1" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>357</v>
+        <v>269</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>358</v>
+        <v>270</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>367</v>
+        <v>271</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>360</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>270</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>362</v>
-      </c>
-      <c r="E3" s="18"/>
+        <v>271</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" s="20"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="21"/>
+      <c r="D6" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3072,31 +2885,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>445</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>446</v>
+      <c r="C1" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>447</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>448</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>449</v>
+      <c r="D2" s="21" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3107,11 +2920,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3679,7 +3492,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>432</v>
+        <v>344</v>
       </c>
       <c r="D39" t="s">
         <v>101</v>
@@ -3687,7 +3500,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>431</v>
+        <v>343</v>
       </c>
       <c r="B40" t="str">
         <f>"1"</f>
@@ -3938,1251 +3751,6 @@
       </c>
       <c r="D56" s="2" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>265</v>
-      </c>
-      <c r="B58" s="15" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>268</v>
-      </c>
-      <c r="D58" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>265</v>
-      </c>
-      <c r="B59" s="15" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C59" t="s">
-        <v>269</v>
-      </c>
-      <c r="D59" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>265</v>
-      </c>
-      <c r="B60" s="15" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C60" t="s">
-        <v>270</v>
-      </c>
-      <c r="D60" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>265</v>
-      </c>
-      <c r="B61" s="15" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
-        <v>271</v>
-      </c>
-      <c r="D61" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>265</v>
-      </c>
-      <c r="B62" s="15" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C62" t="s">
-        <v>272</v>
-      </c>
-      <c r="D62" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>265</v>
-      </c>
-      <c r="B63" s="15" t="str">
-        <f>"6"</f>
-        <v>6</v>
-      </c>
-      <c r="C63" t="s">
-        <v>273</v>
-      </c>
-      <c r="D63" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>265</v>
-      </c>
-      <c r="B64" s="15" t="str">
-        <f>"7"</f>
-        <v>7</v>
-      </c>
-      <c r="C64" t="s">
-        <v>274</v>
-      </c>
-      <c r="D64" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>265</v>
-      </c>
-      <c r="B65" s="15" t="str">
-        <f>"9"</f>
-        <v>9</v>
-      </c>
-      <c r="C65" t="s">
-        <v>275</v>
-      </c>
-      <c r="D65" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>265</v>
-      </c>
-      <c r="B66" s="15" t="str">
-        <f>"10"</f>
-        <v>10</v>
-      </c>
-      <c r="C66" t="s">
-        <v>276</v>
-      </c>
-      <c r="D66" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>265</v>
-      </c>
-      <c r="B67" s="15" t="str">
-        <f>"11"</f>
-        <v>11</v>
-      </c>
-      <c r="C67" t="s">
-        <v>277</v>
-      </c>
-      <c r="D67" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>265</v>
-      </c>
-      <c r="B68" s="15" t="str">
-        <f>"12"</f>
-        <v>12</v>
-      </c>
-      <c r="C68" t="s">
-        <v>278</v>
-      </c>
-      <c r="D68" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>265</v>
-      </c>
-      <c r="B69" s="15" t="str">
-        <f>"13"</f>
-        <v>13</v>
-      </c>
-      <c r="C69" t="s">
-        <v>279</v>
-      </c>
-      <c r="D69" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>265</v>
-      </c>
-      <c r="B70" s="15" t="str">
-        <f>"14"</f>
-        <v>14</v>
-      </c>
-      <c r="C70" t="s">
-        <v>280</v>
-      </c>
-      <c r="D70" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>265</v>
-      </c>
-      <c r="B71" s="15" t="str">
-        <f>"15"</f>
-        <v>15</v>
-      </c>
-      <c r="C71" t="s">
-        <v>281</v>
-      </c>
-      <c r="D71" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>265</v>
-      </c>
-      <c r="B72" s="15" t="str">
-        <f>"16"</f>
-        <v>16</v>
-      </c>
-      <c r="C72" t="s">
-        <v>282</v>
-      </c>
-      <c r="D72" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>265</v>
-      </c>
-      <c r="B73" s="15" t="str">
-        <f>"17"</f>
-        <v>17</v>
-      </c>
-      <c r="C73" t="s">
-        <v>283</v>
-      </c>
-      <c r="D73" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>265</v>
-      </c>
-      <c r="B74" s="15" t="str">
-        <f>"18"</f>
-        <v>18</v>
-      </c>
-      <c r="C74" t="s">
-        <v>284</v>
-      </c>
-      <c r="D74" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>265</v>
-      </c>
-      <c r="B75" s="15" t="str">
-        <f>"19"</f>
-        <v>19</v>
-      </c>
-      <c r="C75" t="s">
-        <v>285</v>
-      </c>
-      <c r="D75" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>265</v>
-      </c>
-      <c r="B76" s="15" t="str">
-        <f>"20"</f>
-        <v>20</v>
-      </c>
-      <c r="C76" t="s">
-        <v>286</v>
-      </c>
-      <c r="D76" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>265</v>
-      </c>
-      <c r="B77" s="15" t="str">
-        <f>"21"</f>
-        <v>21</v>
-      </c>
-      <c r="C77" t="s">
-        <v>287</v>
-      </c>
-      <c r="D77" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>265</v>
-      </c>
-      <c r="B78" s="15" t="str">
-        <f>"22"</f>
-        <v>22</v>
-      </c>
-      <c r="C78" t="s">
-        <v>288</v>
-      </c>
-      <c r="D78" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>265</v>
-      </c>
-      <c r="B79" s="15" t="str">
-        <f>"23"</f>
-        <v>23</v>
-      </c>
-      <c r="C79" t="s">
-        <v>289</v>
-      </c>
-      <c r="D79" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>265</v>
-      </c>
-      <c r="B80" s="15" t="str">
-        <f>"24"</f>
-        <v>24</v>
-      </c>
-      <c r="C80" t="s">
-        <v>290</v>
-      </c>
-      <c r="D80" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>265</v>
-      </c>
-      <c r="B81" s="15" t="str">
-        <f>"25"</f>
-        <v>25</v>
-      </c>
-      <c r="C81" t="s">
-        <v>291</v>
-      </c>
-      <c r="D81" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>265</v>
-      </c>
-      <c r="B82" s="15" t="str">
-        <f>"26"</f>
-        <v>26</v>
-      </c>
-      <c r="C82" t="s">
-        <v>292</v>
-      </c>
-      <c r="D82" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>265</v>
-      </c>
-      <c r="B83" s="15" t="str">
-        <f>"27"</f>
-        <v>27</v>
-      </c>
-      <c r="C83" t="s">
-        <v>293</v>
-      </c>
-      <c r="D83" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>265</v>
-      </c>
-      <c r="B84" s="15" t="str">
-        <f>"28"</f>
-        <v>28</v>
-      </c>
-      <c r="C84" t="s">
-        <v>294</v>
-      </c>
-      <c r="D84" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>265</v>
-      </c>
-      <c r="B85" s="15" t="str">
-        <f>"29"</f>
-        <v>29</v>
-      </c>
-      <c r="C85" t="s">
-        <v>295</v>
-      </c>
-      <c r="D85" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>265</v>
-      </c>
-      <c r="B86" s="15" t="str">
-        <f>"30"</f>
-        <v>30</v>
-      </c>
-      <c r="C86" t="s">
-        <v>296</v>
-      </c>
-      <c r="D86" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>265</v>
-      </c>
-      <c r="B87" s="15" t="str">
-        <f>"31"</f>
-        <v>31</v>
-      </c>
-      <c r="C87" t="s">
-        <v>297</v>
-      </c>
-      <c r="D87" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>265</v>
-      </c>
-      <c r="B88" s="15" t="str">
-        <f>"32"</f>
-        <v>32</v>
-      </c>
-      <c r="C88" t="s">
-        <v>298</v>
-      </c>
-      <c r="D88" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>266</v>
-      </c>
-      <c r="B89" s="15" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="D89" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>266</v>
-      </c>
-      <c r="B90" s="15" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="D90" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>266</v>
-      </c>
-      <c r="B91" s="15" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="D91" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>266</v>
-      </c>
-      <c r="B92" s="15" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="D92" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>266</v>
-      </c>
-      <c r="B93" s="15" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="D93" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>266</v>
-      </c>
-      <c r="B94" s="15" t="str">
-        <f>"6"</f>
-        <v>6</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="D94" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>266</v>
-      </c>
-      <c r="B95" s="15" t="str">
-        <f>"7"</f>
-        <v>7</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="D95" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>266</v>
-      </c>
-      <c r="B96" t="str">
-        <f>"8"</f>
-        <v>8</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="D96" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>266</v>
-      </c>
-      <c r="B97" s="15" t="str">
-        <f>"9"</f>
-        <v>9</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="D97" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>266</v>
-      </c>
-      <c r="B98" s="15" t="str">
-        <f>"10"</f>
-        <v>10</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="D98" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>266</v>
-      </c>
-      <c r="B99" s="15" t="str">
-        <f>"11"</f>
-        <v>11</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="D99" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>266</v>
-      </c>
-      <c r="B100" s="15" t="str">
-        <f>"12"</f>
-        <v>12</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="D100" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>266</v>
-      </c>
-      <c r="B101" s="15" t="str">
-        <f>"13"</f>
-        <v>13</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="D101" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>266</v>
-      </c>
-      <c r="B102" s="15" t="str">
-        <f>"14"</f>
-        <v>14</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="D102" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>266</v>
-      </c>
-      <c r="B103" s="15" t="str">
-        <f>"15"</f>
-        <v>15</v>
-      </c>
-      <c r="C103" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="D103" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>266</v>
-      </c>
-      <c r="B104" s="15" t="str">
-        <f>"16"</f>
-        <v>16</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="D104" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>266</v>
-      </c>
-      <c r="B105" s="15" t="str">
-        <f>"17"</f>
-        <v>17</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="D105" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>266</v>
-      </c>
-      <c r="B106" s="15" t="str">
-        <f>"18"</f>
-        <v>18</v>
-      </c>
-      <c r="C106" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="D106" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>266</v>
-      </c>
-      <c r="B107" s="15" t="str">
-        <f>"19"</f>
-        <v>19</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="D107" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>266</v>
-      </c>
-      <c r="B108" s="15" t="str">
-        <f>"20"</f>
-        <v>20</v>
-      </c>
-      <c r="C108" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="D108" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>266</v>
-      </c>
-      <c r="B109" s="15" t="str">
-        <f>"21"</f>
-        <v>21</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="D109" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>266</v>
-      </c>
-      <c r="B110" s="15" t="str">
-        <f>"22"</f>
-        <v>22</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="D110" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>266</v>
-      </c>
-      <c r="B111" s="15" t="str">
-        <f>"23"</f>
-        <v>23</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="D111" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>266</v>
-      </c>
-      <c r="B112" s="15" t="str">
-        <f>"24"</f>
-        <v>24</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="D112" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>266</v>
-      </c>
-      <c r="B113" s="15" t="str">
-        <f>"25"</f>
-        <v>25</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="D113" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>266</v>
-      </c>
-      <c r="B114" s="15" t="str">
-        <f>"26"</f>
-        <v>26</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="D114" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>267</v>
-      </c>
-      <c r="B115" s="15" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C115" t="s">
-        <v>325</v>
-      </c>
-      <c r="D115" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>267</v>
-      </c>
-      <c r="B116" s="15" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C116" t="s">
-        <v>326</v>
-      </c>
-      <c r="D116" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>267</v>
-      </c>
-      <c r="B117" s="15" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C117" t="s">
-        <v>327</v>
-      </c>
-      <c r="D117" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>267</v>
-      </c>
-      <c r="B118" s="15" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C118" t="s">
-        <v>328</v>
-      </c>
-      <c r="D118" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>267</v>
-      </c>
-      <c r="B119" s="15" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C119" t="s">
-        <v>329</v>
-      </c>
-      <c r="D119" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>267</v>
-      </c>
-      <c r="B120" s="15" t="str">
-        <f>"6"</f>
-        <v>6</v>
-      </c>
-      <c r="C120" t="s">
-        <v>330</v>
-      </c>
-      <c r="D120" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>267</v>
-      </c>
-      <c r="B121" s="15" t="str">
-        <f>"7"</f>
-        <v>7</v>
-      </c>
-      <c r="C121" t="s">
-        <v>331</v>
-      </c>
-      <c r="D121" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>267</v>
-      </c>
-      <c r="B122" t="str">
-        <f>"8"</f>
-        <v>8</v>
-      </c>
-      <c r="C122" t="s">
-        <v>332</v>
-      </c>
-      <c r="D122" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>267</v>
-      </c>
-      <c r="B123" s="15" t="str">
-        <f>"9"</f>
-        <v>9</v>
-      </c>
-      <c r="C123" t="s">
-        <v>333</v>
-      </c>
-      <c r="D123" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>267</v>
-      </c>
-      <c r="B124" s="15" t="str">
-        <f>"10"</f>
-        <v>10</v>
-      </c>
-      <c r="C124" t="s">
-        <v>334</v>
-      </c>
-      <c r="D124" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>267</v>
-      </c>
-      <c r="B125" s="15" t="str">
-        <f>"11"</f>
-        <v>11</v>
-      </c>
-      <c r="C125" t="s">
-        <v>335</v>
-      </c>
-      <c r="D125" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>267</v>
-      </c>
-      <c r="B126" s="15" t="str">
-        <f>"12"</f>
-        <v>12</v>
-      </c>
-      <c r="C126" t="s">
-        <v>336</v>
-      </c>
-      <c r="D126" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>267</v>
-      </c>
-      <c r="B127" s="15" t="str">
-        <f>"13"</f>
-        <v>13</v>
-      </c>
-      <c r="C127" t="s">
-        <v>337</v>
-      </c>
-      <c r="D127" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>267</v>
-      </c>
-      <c r="B128" s="15" t="str">
-        <f>"14"</f>
-        <v>14</v>
-      </c>
-      <c r="C128" t="s">
-        <v>338</v>
-      </c>
-      <c r="D128" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>267</v>
-      </c>
-      <c r="B129" s="15" t="str">
-        <f>"15"</f>
-        <v>15</v>
-      </c>
-      <c r="C129" t="s">
-        <v>339</v>
-      </c>
-      <c r="D129" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>267</v>
-      </c>
-      <c r="B130" s="15" t="str">
-        <f>"16"</f>
-        <v>16</v>
-      </c>
-      <c r="C130" t="s">
-        <v>340</v>
-      </c>
-      <c r="D130" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>267</v>
-      </c>
-      <c r="B131" s="15" t="str">
-        <f>"17"</f>
-        <v>17</v>
-      </c>
-      <c r="C131" t="s">
-        <v>341</v>
-      </c>
-      <c r="D131" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>267</v>
-      </c>
-      <c r="B132" s="15" t="str">
-        <f>"18"</f>
-        <v>18</v>
-      </c>
-      <c r="C132" t="s">
-        <v>342</v>
-      </c>
-      <c r="D132" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>267</v>
-      </c>
-      <c r="B133" s="15" t="str">
-        <f>"19"</f>
-        <v>19</v>
-      </c>
-      <c r="C133" t="s">
-        <v>343</v>
-      </c>
-      <c r="D133" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>267</v>
-      </c>
-      <c r="B134" s="15" t="str">
-        <f>"20"</f>
-        <v>20</v>
-      </c>
-      <c r="C134" t="s">
-        <v>344</v>
-      </c>
-      <c r="D134" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>267</v>
-      </c>
-      <c r="B135" s="15" t="str">
-        <f>"21"</f>
-        <v>21</v>
-      </c>
-      <c r="C135" t="s">
-        <v>345</v>
-      </c>
-      <c r="D135" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>267</v>
-      </c>
-      <c r="B136" s="15" t="str">
-        <f>"22"</f>
-        <v>22</v>
-      </c>
-      <c r="C136" t="s">
-        <v>346</v>
-      </c>
-      <c r="D136" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>267</v>
-      </c>
-      <c r="B137" s="15" t="str">
-        <f>"23"</f>
-        <v>23</v>
-      </c>
-      <c r="C137" t="s">
-        <v>347</v>
-      </c>
-      <c r="D137" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>267</v>
-      </c>
-      <c r="B138" s="15" t="str">
-        <f>"24"</f>
-        <v>24</v>
-      </c>
-      <c r="C138" t="s">
-        <v>348</v>
-      </c>
-      <c r="D138" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>267</v>
-      </c>
-      <c r="B139" s="15" t="str">
-        <f>"25"</f>
-        <v>25</v>
-      </c>
-      <c r="C139" t="s">
-        <v>349</v>
-      </c>
-      <c r="D139" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>267</v>
-      </c>
-      <c r="B140" s="15" t="str">
-        <f>"26"</f>
-        <v>26</v>
-      </c>
-      <c r="C140" t="s">
-        <v>350</v>
-      </c>
-      <c r="D140" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5194,11 +3762,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5232,10 +3800,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>441</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s">
-        <v>430</v>
+        <v>342</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -5265,7 +3833,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>368</v>
+        <v>280</v>
       </c>
       <c r="B6" t="s">
         <v>143</v>
@@ -5287,7 +3855,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>369</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
@@ -5298,10 +3866,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>364</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>342</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -5309,10 +3877,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>261</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>447</v>
+        <v>260</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -5320,10 +3888,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>262</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
+        <v>261</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>359</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -5331,10 +3899,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>262</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -5342,18 +3910,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
         <v>121</v>
@@ -5364,21 +3932,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>439</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -5386,10 +3954,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>351</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>342</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -5397,10 +3965,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -5408,10 +3976,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>229</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -5419,10 +3987,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -5430,10 +3998,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -5441,7 +4009,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -5452,7 +4020,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -5463,10 +4031,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>443</v>
+        <v>202</v>
       </c>
       <c r="B24" t="s">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -5474,10 +4042,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>355</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>342</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -5485,18 +4053,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B27" t="s">
         <v>143</v>
@@ -5507,21 +4075,21 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>447</v>
+        <v>215</v>
+      </c>
+      <c r="B28" t="s">
+        <v>143</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>433</v>
-      </c>
-      <c r="B29" t="s">
-        <v>430</v>
+        <v>140</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>359</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -5529,10 +4097,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>345</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>342</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -5540,10 +4108,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>435</v>
+        <v>147</v>
       </c>
       <c r="B31" t="s">
-        <v>430</v>
+        <v>131</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -5551,10 +4119,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>347</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>342</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -5562,10 +4130,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>436</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
-        <v>430</v>
+        <v>131</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -5573,10 +4141,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>150</v>
+        <v>348</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>342</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -5584,10 +4152,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -5595,7 +4163,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
@@ -5606,7 +4174,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="B37" t="s">
         <v>29</v>
@@ -5617,10 +4185,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>440</v>
+        <v>188</v>
       </c>
       <c r="B38" t="s">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -5628,10 +4196,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>352</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>342</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -5639,10 +4207,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -5650,10 +4218,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>437</v>
+        <v>179</v>
       </c>
       <c r="B41" t="s">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -5661,10 +4229,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>349</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>342</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -5672,10 +4240,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -5683,10 +4251,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -5694,10 +4262,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>231</v>
+        <v>154</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -5705,10 +4273,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>155</v>
+        <v>231</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -5716,10 +4284,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>238</v>
+        <v>155</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -5727,10 +4295,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -5738,10 +4306,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>125</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -5749,10 +4317,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>442</v>
+        <v>205</v>
       </c>
       <c r="B50" t="s">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -5760,10 +4328,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>182</v>
+        <v>354</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>342</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -5771,62 +4339,40 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>438</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>350</v>
+      </c>
+      <c r="B53" t="s">
+        <v>342</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>254</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B58" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="C54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>264</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="C55" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>258</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="C56" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>259</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="C57" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
-        <v>256</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>257</v>
@@ -5835,9 +4381,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>258</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>370</v>
+        <v>259</v>
       </c>
       <c r="B61" s="14" t="s">
         <v>257</v>
@@ -5846,20 +4403,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>371</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="C62" t="b">
-        <v>0</v>
-      </c>
-    </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>372</v>
+      <c r="A63" s="14" t="s">
+        <v>256</v>
       </c>
       <c r="B63" s="14" t="s">
         <v>257</v>
@@ -5868,23 +4414,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>373</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="C64" t="b">
-        <v>0</v>
-      </c>
-    </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>374</v>
+        <v>282</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -5892,10 +4427,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>375</v>
+        <v>283</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -5903,7 +4438,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>376</v>
+        <v>284</v>
       </c>
       <c r="B67" s="14" t="s">
         <v>257</v>
@@ -5914,10 +4449,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>377</v>
+        <v>285</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -5925,10 +4460,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>378</v>
+        <v>286</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -5936,7 +4471,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>379</v>
+        <v>287</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>257</v>
@@ -5947,10 +4482,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>380</v>
+        <v>288</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -5958,10 +4493,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>381</v>
+        <v>289</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -5969,7 +4504,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>382</v>
+        <v>290</v>
       </c>
       <c r="B73" s="14" t="s">
         <v>257</v>
@@ -5980,10 +4515,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>383</v>
+        <v>291</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
@@ -5991,10 +4526,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>384</v>
+        <v>292</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -6002,7 +4537,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>385</v>
+        <v>293</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>257</v>
@@ -6013,10 +4548,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>386</v>
+        <v>294</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -6024,10 +4559,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>387</v>
+        <v>295</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -6035,7 +4570,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>388</v>
+        <v>296</v>
       </c>
       <c r="B79" s="14" t="s">
         <v>257</v>
@@ -6046,10 +4581,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>389</v>
+        <v>297</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
@@ -6057,10 +4592,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>390</v>
+        <v>298</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -6068,7 +4603,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>391</v>
+        <v>299</v>
       </c>
       <c r="B82" s="14" t="s">
         <v>257</v>
@@ -6079,10 +4614,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>392</v>
+        <v>300</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
@@ -6090,10 +4625,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>393</v>
+        <v>301</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
@@ -6101,7 +4636,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>394</v>
+        <v>302</v>
       </c>
       <c r="B85" s="14" t="s">
         <v>257</v>
@@ -6112,10 +4647,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>395</v>
+        <v>303</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -6123,10 +4658,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>396</v>
+        <v>304</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
@@ -6134,7 +4669,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>397</v>
+        <v>305</v>
       </c>
       <c r="B88" s="14" t="s">
         <v>257</v>
@@ -6145,10 +4680,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>398</v>
+        <v>306</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C89" t="b">
         <v>0</v>
@@ -6156,10 +4691,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>399</v>
+        <v>307</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C90" t="b">
         <v>0</v>
@@ -6167,7 +4702,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>400</v>
+        <v>308</v>
       </c>
       <c r="B91" s="14" t="s">
         <v>257</v>
@@ -6178,10 +4713,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>401</v>
+        <v>309</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C92" t="b">
         <v>0</v>
@@ -6189,10 +4724,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>402</v>
+        <v>310</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C93" t="b">
         <v>0</v>
@@ -6200,7 +4735,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>403</v>
+        <v>311</v>
       </c>
       <c r="B94" s="14" t="s">
         <v>257</v>
@@ -6211,10 +4746,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>404</v>
+        <v>312</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C95" t="b">
         <v>0</v>
@@ -6222,10 +4757,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>405</v>
+        <v>313</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C96" t="b">
         <v>0</v>
@@ -6233,7 +4768,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>406</v>
+        <v>314</v>
       </c>
       <c r="B97" s="14" t="s">
         <v>257</v>
@@ -6244,10 +4779,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>407</v>
+        <v>315</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C98" t="b">
         <v>0</v>
@@ -6255,10 +4790,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>408</v>
+        <v>316</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C99" t="b">
         <v>0</v>
@@ -6266,7 +4801,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>409</v>
+        <v>317</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>257</v>
@@ -6277,10 +4812,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>410</v>
+        <v>318</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C101" t="b">
         <v>0</v>
@@ -6288,10 +4823,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>411</v>
+        <v>319</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C102" t="b">
         <v>0</v>
@@ -6299,7 +4834,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>412</v>
+        <v>320</v>
       </c>
       <c r="B103" s="14" t="s">
         <v>257</v>
@@ -6310,10 +4845,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>413</v>
+        <v>321</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C104" t="b">
         <v>0</v>
@@ -6321,10 +4856,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>414</v>
+        <v>322</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C105" t="b">
         <v>0</v>
@@ -6332,7 +4867,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>415</v>
+        <v>323</v>
       </c>
       <c r="B106" s="14" t="s">
         <v>257</v>
@@ -6343,10 +4878,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>416</v>
+        <v>324</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C107" t="b">
         <v>0</v>
@@ -6354,10 +4889,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>417</v>
+        <v>325</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C108" t="b">
         <v>0</v>
@@ -6365,7 +4900,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>418</v>
+        <v>326</v>
       </c>
       <c r="B109" s="14" t="s">
         <v>257</v>
@@ -6376,10 +4911,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>419</v>
+        <v>327</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C110" t="b">
         <v>0</v>
@@ -6387,10 +4922,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>420</v>
+        <v>328</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C111" t="b">
         <v>0</v>
@@ -6398,7 +4933,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>421</v>
+        <v>329</v>
       </c>
       <c r="B112" s="14" t="s">
         <v>257</v>
@@ -6409,10 +4944,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>422</v>
+        <v>330</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C113" t="b">
         <v>0</v>
@@ -6420,10 +4955,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>423</v>
+        <v>331</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C114" t="b">
         <v>0</v>
@@ -6431,7 +4966,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>424</v>
+        <v>332</v>
       </c>
       <c r="B115" s="14" t="s">
         <v>257</v>
@@ -6442,10 +4977,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>425</v>
+        <v>333</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C116" t="b">
         <v>0</v>
@@ -6453,10 +4988,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>426</v>
+        <v>334</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C117" t="b">
         <v>0</v>
@@ -6464,7 +4999,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>427</v>
+        <v>335</v>
       </c>
       <c r="B118" s="14" t="s">
         <v>257</v>
@@ -6475,10 +5010,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>428</v>
+        <v>336</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C119" t="b">
         <v>0</v>
@@ -6486,17 +5021,61 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>429</v>
+        <v>337</v>
       </c>
       <c r="B120" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>338</v>
+      </c>
+      <c r="B121" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="C120" t="b">
+      <c r="C121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>339</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>340</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>341</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C124" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:G93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:G97">
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MUL vaccine + new table for children vaccines
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF/forms/MIF/MIF.xlsx
+++ b/app/config/tables/MIF/forms/MIF/MIF.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3FECA2-79E2-45E5-902C-7878BCE74766}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A20A7A-1018-43B0-934B-B62A07EA6002}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="301">
   <si>
     <t>setting_name</t>
   </si>
@@ -816,186 +816,6 @@
   </si>
   <si>
     <t>ESCO</t>
-  </si>
-  <si>
-    <t>VAC1TIPO</t>
-  </si>
-  <si>
-    <t>VAC1DATA</t>
-  </si>
-  <si>
-    <t>VAC1INF</t>
-  </si>
-  <si>
-    <t>VAC2TIPO</t>
-  </si>
-  <si>
-    <t>VAC2DATA</t>
-  </si>
-  <si>
-    <t>VAC2INF</t>
-  </si>
-  <si>
-    <t>VAC3TIPO</t>
-  </si>
-  <si>
-    <t>VAC3DATA</t>
-  </si>
-  <si>
-    <t>VAC3INF</t>
-  </si>
-  <si>
-    <t>VAC4TIPO</t>
-  </si>
-  <si>
-    <t>VAC4DATA</t>
-  </si>
-  <si>
-    <t>VAC4INF</t>
-  </si>
-  <si>
-    <t>VAC5TIPO</t>
-  </si>
-  <si>
-    <t>VAC5DATA</t>
-  </si>
-  <si>
-    <t>VAC5INF</t>
-  </si>
-  <si>
-    <t>VAC6TIPO</t>
-  </si>
-  <si>
-    <t>VAC6DATA</t>
-  </si>
-  <si>
-    <t>VAC6INF</t>
-  </si>
-  <si>
-    <t>VAC7TIPO</t>
-  </si>
-  <si>
-    <t>VAC7DATA</t>
-  </si>
-  <si>
-    <t>VAC7INF</t>
-  </si>
-  <si>
-    <t>VAC8TIPO</t>
-  </si>
-  <si>
-    <t>VAC8DATA</t>
-  </si>
-  <si>
-    <t>VAC8INF</t>
-  </si>
-  <si>
-    <t>VAC9TIPO</t>
-  </si>
-  <si>
-    <t>VAC9DATA</t>
-  </si>
-  <si>
-    <t>VAC9INF</t>
-  </si>
-  <si>
-    <t>VAC10TIPO</t>
-  </si>
-  <si>
-    <t>VAC10DATA</t>
-  </si>
-  <si>
-    <t>VAC10INF</t>
-  </si>
-  <si>
-    <t>VAC11TIPO</t>
-  </si>
-  <si>
-    <t>VAC11DATA</t>
-  </si>
-  <si>
-    <t>VAC11INF</t>
-  </si>
-  <si>
-    <t>VAC12TIPO</t>
-  </si>
-  <si>
-    <t>VAC12DATA</t>
-  </si>
-  <si>
-    <t>VAC12INF</t>
-  </si>
-  <si>
-    <t>VAC13TIPO</t>
-  </si>
-  <si>
-    <t>VAC13DATA</t>
-  </si>
-  <si>
-    <t>VAC13INF</t>
-  </si>
-  <si>
-    <t>VAC14TIPO</t>
-  </si>
-  <si>
-    <t>VAC14DATA</t>
-  </si>
-  <si>
-    <t>VAC14INF</t>
-  </si>
-  <si>
-    <t>VAC15TIPO</t>
-  </si>
-  <si>
-    <t>VAC15DATA</t>
-  </si>
-  <si>
-    <t>VAC15INF</t>
-  </si>
-  <si>
-    <t>VAC16TIPO</t>
-  </si>
-  <si>
-    <t>VAC16DATA</t>
-  </si>
-  <si>
-    <t>VAC16INF</t>
-  </si>
-  <si>
-    <t>VAC17TIPO</t>
-  </si>
-  <si>
-    <t>VAC17DATA</t>
-  </si>
-  <si>
-    <t>VAC17INF</t>
-  </si>
-  <si>
-    <t>VAC18TIPO</t>
-  </si>
-  <si>
-    <t>VAC18DATA</t>
-  </si>
-  <si>
-    <t>VAC18INF</t>
-  </si>
-  <si>
-    <t>VAC19TIPO</t>
-  </si>
-  <si>
-    <t>VAC19DATA</t>
-  </si>
-  <si>
-    <t>VAC19INF</t>
-  </si>
-  <si>
-    <t>VAC20TIPO</t>
-  </si>
-  <si>
-    <t>VAC20DATA</t>
-  </si>
-  <si>
-    <t>VAC20INF</t>
   </si>
   <si>
     <t>select_multiple</t>
@@ -1581,13 +1401,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>353</v>
+        <v>293</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>350</v>
+        <v>290</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>18</v>
@@ -1641,7 +1461,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>352</v>
+        <v>292</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1707,7 +1527,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>351</v>
+        <v>291</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>11</v>
@@ -1879,7 +1699,7 @@
         <v>216</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>340</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1894,7 +1714,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" s="19" t="s">
-        <v>335</v>
+        <v>275</v>
       </c>
       <c r="F18" t="s">
         <v>135</v>
@@ -1908,13 +1728,13 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E19" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F19" t="s">
-        <v>321</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1922,7 +1742,7 @@
         <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>322</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1992,13 +1812,13 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E28" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F28" t="s">
-        <v>323</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -2052,13 +1872,13 @@
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E34" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F34" t="s">
-        <v>324</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
@@ -2087,10 +1907,10 @@
         <v>149</v>
       </c>
       <c r="G38" t="s">
-        <v>356</v>
+        <v>296</v>
       </c>
       <c r="H38" t="s">
-        <v>354</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
@@ -2101,10 +1921,10 @@
         <v>217</v>
       </c>
       <c r="G39" t="s">
-        <v>357</v>
+        <v>297</v>
       </c>
       <c r="H39" t="s">
-        <v>355</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.25">
@@ -2189,7 +2009,7 @@
         <v>160</v>
       </c>
       <c r="I47" t="s">
-        <v>345</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
@@ -2208,7 +2028,7 @@
         <v>160</v>
       </c>
       <c r="I49" t="s">
-        <v>346</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2237,10 +2057,10 @@
         <v>256</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>341</v>
+        <v>281</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>342</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2248,7 +2068,7 @@
         <v>150</v>
       </c>
       <c r="C54" t="s">
-        <v>338</v>
+        <v>278</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -2261,21 +2081,21 @@
         <v>257</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>343</v>
+        <v>283</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>344</v>
+        <v>284</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E56" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F56" t="s">
-        <v>339</v>
+        <v>279</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2295,7 +2115,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D60" s="19" t="s">
-        <v>335</v>
+        <v>275</v>
       </c>
       <c r="F60" t="s">
         <v>164</v>
@@ -2407,7 +2227,7 @@
         <v>198</v>
       </c>
       <c r="I70" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
@@ -2423,7 +2243,7 @@
         <v>198</v>
       </c>
       <c r="I72" t="s">
-        <v>348</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
@@ -2457,13 +2277,13 @@
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E77" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F77" t="s">
-        <v>325</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
@@ -2482,13 +2302,13 @@
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E79" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F79" t="s">
-        <v>326</v>
+        <v>266</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
@@ -2507,13 +2327,13 @@
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E81" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F81" t="s">
-        <v>327</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -2542,13 +2362,13 @@
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E85" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F85" t="s">
-        <v>328</v>
+        <v>268</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
@@ -2567,13 +2387,13 @@
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E87" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F87" t="s">
-        <v>329</v>
+        <v>269</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
@@ -2681,13 +2501,13 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E99" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="F99" t="s">
-        <v>331</v>
+        <v>271</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -2721,13 +2541,13 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="E104" t="s">
-        <v>358</v>
+        <v>298</v>
       </c>
       <c r="F104" t="s">
-        <v>330</v>
+        <v>270</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -2831,30 +2651,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>332</v>
+        <v>272</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>333</v>
+        <v>273</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>334</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>335</v>
+        <v>275</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>336</v>
+        <v>276</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>134</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>337</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2888,7 +2708,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>353</v>
+        <v>293</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
@@ -3437,7 +3257,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>320</v>
+        <v>260</v>
       </c>
       <c r="D39" t="s">
         <v>96</v>
@@ -3445,7 +3265,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="B40" t="str">
         <f>"1"</f>
@@ -3700,22 +3520,22 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>358</v>
+        <v>298</v>
       </c>
       <c r="B57" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>359</v>
+        <v>299</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>359</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>358</v>
+        <v>298</v>
       </c>
       <c r="B58" t="str">
         <f>"2"</f>
@@ -3740,8 +3560,8 @@
   <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,10 +3595,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>329</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -3841,10 +3661,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>339</v>
+        <v>279</v>
       </c>
       <c r="B9" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -3907,10 +3727,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>327</v>
+        <v>267</v>
       </c>
       <c r="B15" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -3995,10 +3815,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>331</v>
+        <v>271</v>
       </c>
       <c r="B23" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -4042,7 +3862,7 @@
         <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>335</v>
+        <v>275</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -4050,10 +3870,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>321</v>
+        <v>261</v>
       </c>
       <c r="B28" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -4072,10 +3892,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>323</v>
+        <v>263</v>
       </c>
       <c r="B30" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -4094,10 +3914,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>324</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -4149,10 +3969,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>328</v>
+        <v>268</v>
       </c>
       <c r="B37" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -4182,10 +4002,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>325</v>
+        <v>265</v>
       </c>
       <c r="B40" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -4259,7 +4079,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="B47" t="s">
         <v>138</v>
@@ -4270,10 +4090,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>330</v>
+        <v>270</v>
       </c>
       <c r="B48" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -4292,10 +4112,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>326</v>
+        <v>266</v>
       </c>
       <c r="B50" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -4369,7 +4189,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>234</v>
@@ -4390,664 +4210,184 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>258</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C63" t="b">
-        <v>0</v>
-      </c>
+      <c r="B63" s="13"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>259</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C64" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>260</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C65" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>261</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C66" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>262</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C67" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>263</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C68" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>264</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C69" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>265</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C70" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>266</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C71" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>267</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C72" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>268</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>269</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C74" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>270</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>271</v>
-      </c>
-      <c r="B76" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C76" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>272</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C77" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>273</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C78" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>274</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C79" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>275</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C80" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>276</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C81" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>277</v>
-      </c>
-      <c r="B82" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C82" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>278</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C83" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>279</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C84" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>280</v>
-      </c>
-      <c r="B85" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C85" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>281</v>
-      </c>
-      <c r="B86" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C86" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>282</v>
-      </c>
-      <c r="B87" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C87" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>283</v>
-      </c>
-      <c r="B88" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C88" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>284</v>
-      </c>
-      <c r="B89" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C89" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>285</v>
-      </c>
-      <c r="B90" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C90" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>286</v>
-      </c>
-      <c r="B91" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C91" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>287</v>
-      </c>
-      <c r="B92" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C92" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>288</v>
-      </c>
-      <c r="B93" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C93" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>289</v>
-      </c>
-      <c r="B94" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C94" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>290</v>
-      </c>
-      <c r="B95" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C95" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>291</v>
-      </c>
-      <c r="B96" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C96" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>292</v>
-      </c>
-      <c r="B97" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C97" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>293</v>
-      </c>
-      <c r="B98" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C98" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>294</v>
-      </c>
-      <c r="B99" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>295</v>
-      </c>
-      <c r="B100" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C100" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>296</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C101" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>297</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C102" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>298</v>
-      </c>
-      <c r="B103" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C103" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>299</v>
-      </c>
-      <c r="B104" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C104" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>300</v>
-      </c>
-      <c r="B105" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C105" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>301</v>
-      </c>
-      <c r="B106" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C106" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>302</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C107" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>303</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C108" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>304</v>
-      </c>
-      <c r="B109" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C109" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>305</v>
-      </c>
-      <c r="B110" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C110" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>306</v>
-      </c>
-      <c r="B111" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C111" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>307</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C112" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>308</v>
-      </c>
-      <c r="B113" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C113" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>309</v>
-      </c>
-      <c r="B114" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C114" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>310</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C115" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>311</v>
-      </c>
-      <c r="B116" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C116" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>312</v>
-      </c>
-      <c r="B117" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C117" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>313</v>
-      </c>
-      <c r="B118" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C118" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>314</v>
-      </c>
-      <c r="B119" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C119" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>315</v>
-      </c>
-      <c r="B120" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C120" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>316</v>
-      </c>
-      <c r="B121" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C121" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>317</v>
-      </c>
-      <c r="B122" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C122" t="b">
-        <v>0</v>
-      </c>
+      <c r="B64" s="13"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="13"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="13"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="13"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="13"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="13"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="13"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="13"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="13"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="13"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="13"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="13"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="13"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="13"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="13"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="13"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="13"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="13"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="13"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="13"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="13"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="13"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="13"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="13"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="13"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="13"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="13"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="13"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="13"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="13"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="13"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="13"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="13"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="13"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="13"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="13"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="13"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="13"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="13"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="13"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="13"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="13"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="13"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="13"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="13"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="13"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" s="13"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="13"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="13"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="13"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="13"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="13"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="13"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="13"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="13"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="13"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="13"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="13"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C52">

</xml_diff>

<commit_message>
Wokring link between child and mother
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF/forms/MIF/MIF.xlsx
+++ b/app/config/tables/MIF/forms/MIF/MIF.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD930912-BD8F-4A38-BC76-6864D85A5C3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C021C6AC-6F93-492C-8E68-CED80F05C5A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="choices" sheetId="3" r:id="rId5"/>
     <sheet name="model" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1379,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5:D5"/>
     </sheetView>
@@ -3559,7 +3559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>

</xml_diff>

<commit_message>
Added Obstetric history noter til MIF
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF/forms/MIF/MIF.xlsx
+++ b/app/config/tables/MIF/forms/MIF/MIF.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A54F6B-7406-4E70-805F-589C5536CDB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04D3246-ECF9-424E-B1E7-D02AEA2FB252}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="302">
   <si>
     <t>setting_name</t>
   </si>
@@ -1489,11 +1489,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:R105"/>
+  <dimension ref="A1:R110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,112 +2266,109 @@
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>24</v>
-      </c>
-      <c r="F76" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="G76" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="H76" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>256</v>
-      </c>
-      <c r="E77" t="s">
-        <v>257</v>
+        <v>24</v>
       </c>
       <c r="F77" t="s">
-        <v>263</v>
+        <v>169</v>
+      </c>
+      <c r="G77" t="s">
+        <v>170</v>
+      </c>
+      <c r="H77" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>24</v>
+        <v>256</v>
+      </c>
+      <c r="E78" t="s">
+        <v>257</v>
       </c>
       <c r="F78" t="s">
-        <v>172</v>
-      </c>
-      <c r="G78" t="s">
-        <v>173</v>
-      </c>
-      <c r="H78" t="s">
-        <v>174</v>
+        <v>263</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>256</v>
-      </c>
-      <c r="E79" t="s">
-        <v>257</v>
+        <v>24</v>
       </c>
       <c r="F79" t="s">
-        <v>264</v>
+        <v>172</v>
+      </c>
+      <c r="G79" t="s">
+        <v>173</v>
+      </c>
+      <c r="H79" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>24</v>
+        <v>256</v>
+      </c>
+      <c r="E80" t="s">
+        <v>257</v>
       </c>
       <c r="F80" t="s">
-        <v>175</v>
-      </c>
-      <c r="G80" t="s">
-        <v>176</v>
-      </c>
-      <c r="H80" t="s">
-        <v>177</v>
+        <v>264</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
+        <v>24</v>
+      </c>
+      <c r="F81" t="s">
+        <v>175</v>
+      </c>
+      <c r="G81" t="s">
+        <v>176</v>
+      </c>
+      <c r="H81" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
         <v>256</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E82" t="s">
         <v>257</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F82" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>24</v>
-      </c>
-      <c r="F84" t="s">
-        <v>178</v>
-      </c>
-      <c r="G84" t="s">
-        <v>182</v>
-      </c>
-      <c r="H84" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>256</v>
-      </c>
-      <c r="E85" t="s">
-        <v>257</v>
-      </c>
-      <c r="F85" t="s">
-        <v>266</v>
+        <v>201</v>
+      </c>
+      <c r="G85" t="s">
+        <v>203</v>
+      </c>
+      <c r="H85" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
@@ -2379,13 +2376,13 @@
         <v>24</v>
       </c>
       <c r="F86" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G86" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H86" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -2396,166 +2393,224 @@
         <v>257</v>
       </c>
       <c r="F87" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>24</v>
+      </c>
+      <c r="F88" t="s">
+        <v>180</v>
+      </c>
+      <c r="G88" t="s">
+        <v>183</v>
+      </c>
+      <c r="H88" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>256</v>
+      </c>
+      <c r="E89" t="s">
+        <v>257</v>
+      </c>
+      <c r="F89" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D90" t="s">
-        <v>138</v>
-      </c>
-      <c r="E90" t="s">
-        <v>29</v>
-      </c>
-      <c r="F90" t="s">
-        <v>184</v>
-      </c>
-      <c r="G90" t="s">
-        <v>185</v>
-      </c>
-      <c r="H90" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>150</v>
-      </c>
-      <c r="C91" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
-        <v>126</v>
-      </c>
-      <c r="F92" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="G92" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="H92" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>155</v>
+      <c r="D93" t="s">
+        <v>138</v>
+      </c>
+      <c r="E93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" t="s">
+        <v>184</v>
+      </c>
+      <c r="G93" t="s">
+        <v>185</v>
+      </c>
+      <c r="H93" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>13</v>
+        <v>150</v>
+      </c>
+      <c r="C94" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>12</v>
+      <c r="D95" t="s">
+        <v>126</v>
+      </c>
+      <c r="F95" t="s">
+        <v>187</v>
+      </c>
+      <c r="G95" t="s">
+        <v>188</v>
+      </c>
+      <c r="H95" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
-        <v>138</v>
-      </c>
-      <c r="E96" t="s">
-        <v>29</v>
-      </c>
-      <c r="F96" t="s">
-        <v>190</v>
-      </c>
-      <c r="G96" t="s">
-        <v>191</v>
-      </c>
-      <c r="H96" t="s">
-        <v>251</v>
+      <c r="B96" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>150</v>
-      </c>
-      <c r="C97" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
-        <v>24</v>
-      </c>
-      <c r="F98" t="s">
-        <v>192</v>
-      </c>
-      <c r="G98" t="s">
-        <v>193</v>
-      </c>
-      <c r="H98" t="s">
-        <v>194</v>
+      <c r="B98" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>256</v>
-      </c>
-      <c r="E99" t="s">
-        <v>257</v>
-      </c>
-      <c r="F99" t="s">
-        <v>269</v>
+        <v>201</v>
+      </c>
+      <c r="G99" t="s">
+        <v>203</v>
+      </c>
+      <c r="H99" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>155</v>
+      <c r="D100" t="s">
+        <v>138</v>
+      </c>
+      <c r="E100" t="s">
+        <v>29</v>
+      </c>
+      <c r="F100" t="s">
+        <v>190</v>
+      </c>
+      <c r="G100" t="s">
+        <v>191</v>
+      </c>
+      <c r="H100" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>13</v>
+        <v>150</v>
+      </c>
+      <c r="C101" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>12</v>
+      <c r="D102" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" t="s">
+        <v>192</v>
+      </c>
+      <c r="G102" t="s">
+        <v>193</v>
+      </c>
+      <c r="H102" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
+        <v>256</v>
+      </c>
+      <c r="E103" t="s">
+        <v>257</v>
+      </c>
+      <c r="F103" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>201</v>
+      </c>
+      <c r="G107" t="s">
+        <v>203</v>
+      </c>
+      <c r="H107" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
         <v>24</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F108" t="s">
         <v>195</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G108" t="s">
         <v>197</v>
       </c>
-      <c r="H103" t="s">
+      <c r="H108" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
         <v>256</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E109" t="s">
         <v>296</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F109" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="10"/>
-      <c r="B105" t="s">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="10"/>
+      <c r="B110" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3562,7 +3617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>

</xml_diff>